<commit_message>
Updated geometry to follow the original design more closely
</commit_message>
<xml_diff>
--- a/docs/SwissRailwayClockNumbers.xlsx
+++ b/docs/SwissRailwayClockNumbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahugg\Source\SwissRailwayClock\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D955C3-9189-4608-B814-D5C6C08ADBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBECC22-8B57-47C0-8FEA-7A78E9ADD682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{32F3F340-B50A-468F-A7CD-79062FF14C1B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="18">
   <si>
     <t>bigTickMark</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Difference</t>
+  </si>
+  <si>
+    <t>Pixels based on Original design</t>
+  </si>
+  <si>
+    <t>Original design</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBC2821-D5E0-4A7F-9CB8-332B59F2C856}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +478,7 @@
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>11</v>
       </c>
@@ -483,7 +489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -530,22 +536,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>9.5500000000000007</v>
+        <f>2*9.55</f>
+        <v>19.100000000000001</v>
       </c>
       <c r="H3">
         <f>B3/$B$3</f>
         <v>1</v>
       </c>
       <c r="N3">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -563,19 +570,19 @@
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I8" si="0">C4/$B$3</f>
-        <v>0.23036649214659685</v>
+        <v>0.11518324607329843</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J8" si="1">D4/$B$3</f>
-        <v>6.8062827225130892E-2</v>
+        <v>3.4031413612565446E-2</v>
       </c>
       <c r="K4">
         <f t="shared" ref="J4:K8" si="2">E4/$B$3</f>
-        <v>6.8062827225130892E-2</v>
+        <v>3.4031413612565446E-2</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L8" si="3">F4/$B$3</f>
-        <v>0.706806282722513</v>
+        <v>0.3534031413612565</v>
       </c>
       <c r="O4">
         <f>ROUND($N$3*I4,0)</f>
@@ -593,8 +600,20 @@
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U4">
+        <v>30</v>
+      </c>
+      <c r="V4">
+        <v>9</v>
+      </c>
+      <c r="W4">
+        <v>9</v>
+      </c>
+      <c r="X4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -612,19 +631,19 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>6.8062827225130892E-2</v>
+        <v>3.4031413612565446E-2</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>2.6178010471204185E-2</v>
+        <v>1.3089005235602092E-2</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>2.6178010471204185E-2</v>
+        <v>1.3089005235602092E-2</v>
       </c>
       <c r="L5">
         <f t="shared" si="3"/>
-        <v>0.86910994764397909</v>
+        <v>0.43455497382198954</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:O8" si="5">ROUND($N$3*I5,0)</f>
@@ -642,8 +661,20 @@
         <f t="shared" ref="R5:S8" si="8">ROUND($N$3*L5,0)</f>
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U5">
+        <v>9</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -661,19 +692,19 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0.8481675392670156</v>
+        <v>0.4240837696335078</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>0.1256544502617801</v>
+        <v>6.2827225130890049E-2</v>
       </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>9.947643979057591E-2</v>
+        <v>4.9738219895287955E-2</v>
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>-0.23036649214659685</v>
+        <v>-0.11518324607329843</v>
       </c>
       <c r="O6">
         <f t="shared" si="5"/>
@@ -691,8 +722,20 @@
         <f t="shared" si="8"/>
         <v>-30</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <v>110</v>
+      </c>
+      <c r="V6">
+        <v>16</v>
+      </c>
+      <c r="W6">
+        <v>13</v>
+      </c>
+      <c r="X6">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -710,19 +753,19 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.12565445026178</v>
+        <v>0.56282722513089001</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>0.10471204188481674</v>
+        <v>5.235602094240837E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>7.3298429319371722E-2</v>
+        <v>3.6649214659685861E-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
-        <v>-0.23560209424083767</v>
+        <v>-0.11780104712041883</v>
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
@@ -740,8 +783,20 @@
         <f t="shared" si="8"/>
         <v>-31</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <v>146</v>
+      </c>
+      <c r="V7">
+        <v>14</v>
+      </c>
+      <c r="W7">
+        <v>10</v>
+      </c>
+      <c r="X7">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -762,23 +817,23 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0.93717277486910977</v>
+        <v>0.46858638743455489</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>3.1413612565445025E-2</v>
+        <v>1.5706806282722512E-2</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>3.1413612565445025E-2</v>
+        <v>1.5706806282722512E-2</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>-0.32460732984293195</v>
+        <v>-0.16230366492146597</v>
       </c>
       <c r="M8">
         <f t="shared" ref="M8" si="9">G8/$B$3</f>
-        <v>9.947643979057591E-2</v>
+        <v>4.9738219895287955E-2</v>
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
@@ -800,13 +855,46 @@
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U8">
+        <v>122</v>
+      </c>
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <v>-42</v>
+      </c>
+      <c r="Y8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>5</v>
       </c>
@@ -838,7 +926,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
       <c r="H12">
         <v>4</v>
       </c>
@@ -848,22 +942,37 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3.5</v>
+      </c>
+      <c r="E13">
+        <v>3.5</v>
+      </c>
+      <c r="F13">
+        <v>36.5</v>
+      </c>
       <c r="I13" s="3">
         <f t="shared" ref="I13:L17" si="10">ROUND(I4,$H$12)</f>
-        <v>0.23039999999999999</v>
+        <v>0.1152</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="10"/>
-        <v>6.8099999999999994E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="10"/>
-        <v>6.8099999999999994E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="L13" s="3">
         <f t="shared" si="10"/>
-        <v>0.70679999999999998</v>
+        <v>0.35339999999999999</v>
       </c>
       <c r="M13" s="1"/>
       <c r="O13">
@@ -883,22 +992,37 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>3.5</v>
+      </c>
+      <c r="D14">
+        <v>1.4</v>
+      </c>
+      <c r="E14">
+        <v>1.4</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
       <c r="I14" s="3">
         <f t="shared" si="10"/>
-        <v>6.8099999999999994E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="10"/>
-        <v>2.6200000000000001E-2</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="10"/>
-        <v>2.6200000000000001E-2</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="10"/>
-        <v>0.86909999999999998</v>
+        <v>0.43459999999999999</v>
       </c>
       <c r="M14" s="1"/>
       <c r="O14">
@@ -918,22 +1042,37 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F15">
+        <v>-12</v>
+      </c>
       <c r="I15" s="1">
         <f t="shared" si="10"/>
-        <v>0.84819999999999995</v>
+        <v>0.42409999999999998</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="10"/>
-        <v>0.12570000000000001</v>
+        <v>6.2799999999999995E-2</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="10"/>
-        <v>9.9500000000000005E-2</v>
+        <v>4.9700000000000001E-2</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="10"/>
-        <v>-0.23039999999999999</v>
+        <v>-0.1152</v>
       </c>
       <c r="M15" s="1"/>
       <c r="O15">
@@ -953,22 +1092,37 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>57.8</v>
+      </c>
+      <c r="D16">
+        <v>5.2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="F16">
+        <v>-12</v>
+      </c>
       <c r="I16" s="1">
         <f t="shared" si="10"/>
-        <v>1.1256999999999999</v>
+        <v>0.56279999999999997</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="10"/>
-        <v>0.1047</v>
+        <v>5.2400000000000002E-2</v>
       </c>
       <c r="K16" s="1">
         <f t="shared" si="10"/>
-        <v>7.3300000000000004E-2</v>
+        <v>3.6600000000000001E-2</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="10"/>
-        <v>-0.2356</v>
+        <v>-0.1178</v>
       </c>
       <c r="M16" s="1"/>
       <c r="O16">
@@ -988,26 +1142,44 @@
         <v>-31</v>
       </c>
     </row>
-    <row r="17" spans="9:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>47.9</v>
+      </c>
+      <c r="D17">
+        <v>1.4</v>
+      </c>
+      <c r="E17">
+        <v>1.4</v>
+      </c>
+      <c r="F17">
+        <v>-16.5</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="I17" s="3">
         <f t="shared" si="10"/>
-        <v>0.93720000000000003</v>
+        <v>0.46860000000000002</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="10"/>
-        <v>3.1399999999999997E-2</v>
+        <v>1.5699999999999999E-2</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="10"/>
-        <v>3.1399999999999997E-2</v>
+        <v>1.5699999999999999E-2</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="10"/>
-        <v>-0.3246</v>
+        <v>-0.1623</v>
       </c>
       <c r="M17" s="3">
         <f>ROUND(M8,$H$12)</f>
-        <v>9.9500000000000005E-2</v>
+        <v>4.9700000000000001E-2</v>
       </c>
       <c r="O17">
         <f t="shared" si="12"/>
@@ -1030,12 +1202,48 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="9:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
       <c r="N19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="9:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
       <c r="O20" t="s">
         <v>5</v>
       </c>
@@ -1052,98 +1260,428 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="9:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>ROUND($B$21/$B$12*C13,0)</f>
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:F22" si="16">ROUND($B$21/$B$12*D13,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="16"/>
+        <v>95</v>
+      </c>
+      <c r="I22">
+        <f>C22-O13</f>
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:L22" si="17">D22-P13</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
       <c r="O22">
         <f>O4-O13</f>
         <v>0</v>
       </c>
       <c r="P22">
-        <f t="shared" ref="P22:R22" si="16">P4-P13</f>
+        <f t="shared" ref="P22:R22" si="18">P4-P13</f>
         <v>0</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="R22">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="9:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:F23" si="19">ROUND($B$21/$B$12*C14,0)</f>
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="19"/>
+        <v>117</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I26" si="20">C23-O14</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:J26" si="21">D23-P14</f>
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="K23:K26" si="22">E23-Q14</f>
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23:M26" si="23">F23-R14</f>
+        <v>4</v>
+      </c>
       <c r="O23">
-        <f t="shared" ref="O23:R23" si="17">O5-O14</f>
+        <f t="shared" ref="O23:R23" si="24">O5-O14</f>
         <v>0</v>
       </c>
       <c r="P23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="R23">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="9:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:F24" si="25">ROUND($B$21/$B$12*C15,0)</f>
+        <v>114</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="25"/>
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="25"/>
+        <v>13</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="25"/>
+        <v>-31</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="23"/>
+        <v>-1</v>
+      </c>
       <c r="O24">
-        <f t="shared" ref="O24:R24" si="18">O6-O15</f>
+        <f t="shared" ref="O24:R24" si="26">O6-O15</f>
         <v>0</v>
       </c>
       <c r="P24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="R24">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="9:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:F25" si="27">ROUND($B$21/$B$12*C16,0)</f>
+        <v>150</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="27"/>
+        <v>14</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="27"/>
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="27"/>
+        <v>-31</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
       <c r="O25">
-        <f t="shared" ref="O25:R25" si="19">O7-O16</f>
+        <f t="shared" ref="O25:R25" si="28">O7-O16</f>
         <v>0</v>
       </c>
       <c r="P25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="R25">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="9:19" x14ac:dyDescent="0.3">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:G26" si="29">ROUND($B$21/$B$12*C17,0)</f>
+        <v>125</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="29"/>
+        <v>-43</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="29"/>
+        <v>13</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="23"/>
+        <v>-1</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
       <c r="O26">
-        <f t="shared" ref="O26:S26" si="20">O8-O17</f>
+        <f t="shared" ref="O26:S26" si="30">O8-O17</f>
         <v>0</v>
       </c>
       <c r="P26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="S26">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>ROUND($B$30/$B$12*C13,2)</f>
+        <v>31.2</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:F31" si="31">ROUND($B$30/$B$12*D13,2)</f>
+        <v>9.1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="31"/>
+        <v>9.1</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="31"/>
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:F32" si="32">ROUND($B$30/$B$12*C14,2)</f>
+        <v>9.1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="32"/>
+        <v>3.64</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="32"/>
+        <v>3.64</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="32"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:F33" si="33">ROUND($B$30/$B$12*C15,2)</f>
+        <v>114.4</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="33"/>
+        <v>16.38</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="33"/>
+        <v>13.26</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="33"/>
+        <v>-31.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:F34" si="34">ROUND($B$30/$B$12*C16,2)</f>
+        <v>150.28</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="34"/>
+        <v>13.52</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="34"/>
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="34"/>
+        <v>-31.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:G35" si="35">ROUND($B$30/$B$12*C17,2)</f>
+        <v>124.54</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="35"/>
+        <v>3.64</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="35"/>
+        <v>3.64</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="35"/>
+        <v>-42.9</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="35"/>
+        <v>13.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>